<commit_message>
Pwr failure/restore message added
</commit_message>
<xml_diff>
--- a/HandyDevices/VaultKeeper/VaultKeeper.xlsx
+++ b/HandyDevices/VaultKeeper/VaultKeeper.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sim cards" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Vcc</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>+7 917 571 4318</t>
+  </si>
+  <si>
+    <t>A710720A45E6FA74353AC4C4596597F4F49D1D36</t>
+  </si>
+  <si>
+    <t>Host Key</t>
   </si>
 </sst>
 </file>
@@ -567,20 +573,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
@@ -593,8 +601,11 @@
       <c r="D1" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -605,7 +616,7 @@
         <v>37185130</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -614,6 +625,9 @@
       </c>
       <c r="D3">
         <v>25197333</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>